<commit_message>
Testing bitwise operations & document update
</commit_message>
<xml_diff>
--- a/GBA_Visuals.xlsx
+++ b/GBA_Visuals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Desktop\GBA_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5BB24D6-E9AD-47CD-B2E1-66D03A6F44C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29B683A-217B-463A-A76E-ABF5D40EF12D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FDE2BA73-A3FE-4FEE-8F9E-B561CB09C932}"/>
+    <workbookView xWindow="13500" yWindow="810" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{FDE2BA73-A3FE-4FEE-8F9E-B561CB09C932}"/>
   </bookViews>
   <sheets>
     <sheet name="Letter'A'" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>0x6000c38</t>
   </si>
@@ -105,9 +105,6 @@
     <t>0x600039e</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>0x6000381</t>
   </si>
   <si>
@@ -123,15 +120,9 @@
     <t>0x6000389</t>
   </si>
   <si>
-    <t>0x30008b</t>
-  </si>
-  <si>
     <t>0x600038d</t>
   </si>
   <si>
-    <t>0x60008f</t>
-  </si>
-  <si>
     <t>0x6000391</t>
   </si>
   <si>
@@ -157,13 +148,182 @@
   </si>
   <si>
     <t xml:space="preserve">Changing the address to a 'full address' such as 0x6000380, will place a single pixel in that space. However, entering 0x6000381, will keep the original pixel as well as shade in the next two pixels a long, leaving the middle on empty. </t>
+  </si>
+  <si>
+    <t>0x300038b</t>
+  </si>
+  <si>
+    <t>0x600038f</t>
+  </si>
+  <si>
+    <t>However, using bitshifting on the 'ptr[0] = 0b0001 &lt;&lt; 4' will fill in the second pixel. Using 'ptr[0] = 0b0001 &lt;&lt; 12' will fill in the 4th pixel.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">unsigned int* ptr = (unsigned int*)0x6000380 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Changing the last value, fills in a different pixel which can be seen below.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">ptr[0] = 0b0001 &lt;&lt; 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Fills in the second pixel</t>
+    </r>
+  </si>
+  <si>
+    <t>ptr[0] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[0] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[0] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[0] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>ptr[1] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[1] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[1] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[1] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>ptr[2] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[2] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[2] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[2] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>ptr[3] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[3] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[3] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[3] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>ptr[4] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[4] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[4] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[4] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>ptr[5] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[5] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[5] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[5] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>ptr[6] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[6] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[6] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[6] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>ptr[7] = 0b0001 &lt;&lt; 4</t>
+  </si>
+  <si>
+    <t>ptr[7] = 0b0001 &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t>ptr[7] = 0b0001 &lt;&lt; 20</t>
+  </si>
+  <si>
+    <t>ptr[7] = 0b0001 &lt;&lt; 28</t>
+  </si>
+  <si>
+    <t>0 - 3</t>
+  </si>
+  <si>
+    <t>4 - 7</t>
+  </si>
+  <si>
+    <t>8 - 11</t>
+  </si>
+  <si>
+    <t>12 - 15</t>
+  </si>
+  <si>
+    <t>16 - 19</t>
+  </si>
+  <si>
+    <t>20 - 23</t>
+  </si>
+  <si>
+    <t>24 - 27</t>
+  </si>
+  <si>
+    <t>28 - 31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +355,18 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -232,17 +404,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -259,6 +449,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>418981</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>285619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30E82CD0-6FEB-439D-9A24-67A6A77AB2F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6210300" y="1924050"/>
+          <a:ext cx="952381" cy="1047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266304</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>257150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2AD5A60-AB4E-43F5-A223-E624E4817A4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7210425" y="2295525"/>
+          <a:ext cx="3171429" cy="200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51DD90FA-1860-47D1-8F0A-6A04A4EB11CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6191250" y="904875"/>
+          <a:ext cx="1000000" cy="1057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>285356</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104749</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D0935B2-5FD9-4FB7-B29F-108A0B442AF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7248525" y="1238250"/>
+          <a:ext cx="3152381" cy="209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -669,303 +1040,357 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FA57E1-D692-4F44-9395-E8EB46BEDCA9}">
-  <dimension ref="C2:S9"/>
+  <dimension ref="C2:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:S2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.42578125" style="3"/>
+    <col min="1" max="2" width="8.42578125" style="2"/>
+    <col min="3" max="10" width="10.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+    </row>
+    <row r="6" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="F6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+    </row>
+    <row r="7" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="F12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-    </row>
-    <row r="9" spans="3:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="J12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="L8:S8"/>
-    <mergeCell ref="L9:S9"/>
-    <mergeCell ref="L2:S2"/>
-    <mergeCell ref="L3:S3"/>
-    <mergeCell ref="L4:S4"/>
+  <mergeCells count="6">
+    <mergeCell ref="L11:S11"/>
+    <mergeCell ref="L12:S12"/>
+    <mergeCell ref="L6:S10"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
     <mergeCell ref="L5:S5"/>
-    <mergeCell ref="L6:S6"/>
-    <mergeCell ref="L7:S7"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>